<commit_message>
AC5 Engenharia de requisitos e AC4 desenvolvimento de aplicações distribuídas
</commit_message>
<xml_diff>
--- a/17 - Analise dos Eventos para cada cenario.xlsx
+++ b/17 - Analise dos Eventos para cada cenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/edf52c4709d3657a/FACULDADE/3Semestre/OPE_1/2_Conjunto de Artefatos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/edf52c4709d3657a/FACULDADE/3Semestre/OPE_1/AC05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="11_AD4D361C20488DEA4E38A070FC5866665ADEDD84" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{16558895-7E3A-4768-B318-CAC23642AAEB}"/>
+  <xr:revisionPtr revIDLastSave="366" documentId="11_AD4D361C20488DEA4E38A070FC5866665ADEDD84" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{64697D88-ED18-4C47-92A5-B62A4D879AE2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9195" yWindow="6885" windowWidth="18525" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1 (2)" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>Previsível</t>
   </si>
@@ -206,13 +206,43 @@
     <t>Cliente solicita cancelamento</t>
   </si>
   <si>
-    <t>Atendimento ajusta orçamento</t>
-  </si>
-  <si>
     <t>x(11)</t>
   </si>
   <si>
     <t>Cancelamento de Serviço</t>
+  </si>
+  <si>
+    <t>Atendente ajusta orçamento</t>
+  </si>
+  <si>
+    <t>Atendente agenda Ordem de Serviço</t>
+  </si>
+  <si>
+    <t>Técnico Prepara Ordem de Serviço</t>
+  </si>
+  <si>
+    <t>Técnico executa Ordem de Serviço</t>
+  </si>
+  <si>
+    <t>Cliente retorna confirmação</t>
+  </si>
+  <si>
+    <t>Realização de Serviço</t>
+  </si>
+  <si>
+    <t>x(13)</t>
+  </si>
+  <si>
+    <t>x(14)</t>
+  </si>
+  <si>
+    <t>x(15)</t>
+  </si>
+  <si>
+    <t>x(17)</t>
+  </si>
+  <si>
+    <t>Cliente paga 1ª parcela do Serviço</t>
   </si>
 </sst>
 </file>
@@ -262,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -335,11 +365,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -380,15 +439,33 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -396,12 +473,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74DC250-0219-43E3-99A2-68E9010B61E7}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,24 +775,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1"/>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="E1" s="15" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
@@ -742,7 +815,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -764,8 +837,8 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="17"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="4">
         <f>C3+1</f>
         <v>2</v>
@@ -783,8 +856,8 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="4">
@@ -804,8 +877,8 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -823,8 +896,8 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -842,8 +915,8 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -861,8 +934,8 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -880,8 +953,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -899,8 +972,8 @@
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -918,8 +991,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -937,8 +1010,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>58</v>
+      <c r="A13" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>30</v>
@@ -959,7 +1032,7 @@
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="14" t="s">
         <v>31</v>
       </c>
@@ -967,25 +1040,122 @@
         <v>12</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
     </row>
+    <row r="15" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4">
+        <v>13</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="4">
+        <v>14</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="4">
+        <v>15</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="4">
+        <v>17</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="4">
+        <v>16</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="E1:F1"/>
+  <mergeCells count="9">
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B12"/>
     <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1018,15 +1188,15 @@
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1056,7 +1226,7 @@
       <c r="A3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="4">
@@ -1075,8 +1245,8 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="4">
         <f>C3+1</f>
         <v>2</v>
@@ -1094,8 +1264,8 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="4">
         <f t="shared" ref="C5:C18" si="0">C4+1</f>
         <v>3</v>
@@ -1113,8 +1283,8 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1132,8 +1302,8 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1151,8 +1321,8 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1170,8 +1340,8 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1189,8 +1359,8 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1208,8 +1378,8 @@
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1227,8 +1397,8 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1246,8 +1416,8 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1265,7 +1435,7 @@
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="16" t="s">
         <v>31</v>
       </c>
@@ -1286,8 +1456,8 @@
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1305,8 +1475,8 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1324,7 +1494,7 @@
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -1347,7 +1517,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="9" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Artefatos para entrega de AC05
</commit_message>
<xml_diff>
--- a/17 - Analise dos Eventos para cada cenario.xlsx
+++ b/17 - Analise dos Eventos para cada cenario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/edf52c4709d3657a/FACULDADE/3Semestre/OPE_1/AC05/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Desktop\PASTA COM GIT PARA OPE_TAKAI\GH_Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="11_AD4D361C20488DEA4E38A070FC5866665ADEDD84" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{64697D88-ED18-4C47-92A5-B62A4D879AE2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0996E1-43E1-4C84-9505-D3CCFADB0288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9195" yWindow="6885" windowWidth="18525" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4125" windowWidth="18525" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1 (2)" sheetId="2" r:id="rId1"/>
@@ -439,17 +439,23 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,12 +467,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -757,7 +757,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,26 +775,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="23" t="s">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
@@ -815,7 +815,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -837,8 +837,8 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="4">
         <f>C3+1</f>
         <v>2</v>
@@ -856,8 +856,8 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="18" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="4">
@@ -877,8 +877,8 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -896,8 +896,8 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -915,8 +915,8 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -934,8 +934,8 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -953,8 +953,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -972,8 +972,8 @@
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -991,8 +991,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1010,7 +1010,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -1032,7 +1032,7 @@
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="14" t="s">
         <v>31</v>
       </c>
@@ -1052,7 +1052,7 @@
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="18" t="s">
         <v>63</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -1074,8 +1074,8 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="4">
         <v>14</v>
       </c>
@@ -1092,8 +1092,8 @@
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="4">
         <v>15</v>
       </c>
@@ -1110,8 +1110,8 @@
       <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="17"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="4">
         <v>17</v>
       </c>
@@ -1128,8 +1128,8 @@
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="4">
         <v>16</v>
       </c>
@@ -1188,15 +1188,15 @@
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1226,7 +1226,7 @@
       <c r="A3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="4">
@@ -1245,8 +1245,8 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="4">
         <f>C3+1</f>
         <v>2</v>
@@ -1264,8 +1264,8 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="4">
         <f t="shared" ref="C5:C18" si="0">C4+1</f>
         <v>3</v>
@@ -1283,8 +1283,8 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1302,8 +1302,8 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1321,8 +1321,8 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1340,8 +1340,8 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1359,8 +1359,8 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1378,8 +1378,8 @@
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1397,8 +1397,8 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1416,8 +1416,8 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1435,7 +1435,7 @@
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="16" t="s">
         <v>31</v>
       </c>
@@ -1456,8 +1456,8 @@
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1475,8 +1475,8 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
         <v>14</v>

</xml_diff>

<commit_message>
Alteração pós feedback AC 5
</commit_message>
<xml_diff>
--- a/17 - Analise dos Eventos para cada cenario.xlsx
+++ b/17 - Analise dos Eventos para cada cenario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Desktop\PASTA COM GIT PARA OPE_TAKAI\GH_Team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Desktop\GH_Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0996E1-43E1-4C84-9505-D3CCFADB0288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E7425B-D7BF-4966-86DF-1765355BFFF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4125" windowWidth="18525" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1 (2)" sheetId="2" r:id="rId1"/>
@@ -215,9 +215,6 @@
     <t>Atendente ajusta orçamento</t>
   </si>
   <si>
-    <t>Atendente agenda Ordem de Serviço</t>
-  </si>
-  <si>
     <t>Técnico Prepara Ordem de Serviço</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>Cliente paga 1ª parcela do Serviço</t>
+  </si>
+  <si>
+    <t>Cliente informa data e hora compatível</t>
   </si>
 </sst>
 </file>
@@ -757,7 +757,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="15" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>30</v>
@@ -1062,7 +1062,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
@@ -1080,12 +1080,12 @@
         <v>14</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1098,12 +1098,12 @@
         <v>15</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1116,10 +1116,10 @@
         <v>17</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="6"/>
@@ -1134,12 +1134,12 @@
         <v>16</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>

</xml_diff>